<commit_message>
Implementa regras 0-8 no modo analise e celulas em branco
</commit_message>
<xml_diff>
--- a/Planilha Base de Teste.xlsx
+++ b/Planilha Base de Teste.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Programs - Dados/Projetos/Preenche Planilhas/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE89723D-A613-B642-A01F-B1E697D98691}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D570D9C6-5D5D-1444-8758-7A8184D09DB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="63">
   <si>
     <t>ANÁLISE DOS ELEMENTOS DO PLANO DE APLICAÇÃO</t>
   </si>
@@ -101,9 +101,6 @@
     <t>O indicador geral de resultado é capaz de mensurar o atingimento da Meta Geral?</t>
   </si>
   <si>
-    <t>Redução da taxa estadual de Morte Violenta Intencional para no máximo de 6,41 por 100 mil habitantes até 2027. A taxa atual é de 8,41 mortes por grupo de 100 mil habitantes em 2024, segundo dados do SINESP.</t>
-  </si>
-  <si>
     <t>SIM, pois foi estabelecida uma meta geral que reflete o problema público e demonstrada uma estratégia adequada para a sua mitigação.</t>
   </si>
   <si>
@@ -122,9 +119,6 @@
     <t>Fórmula / Referência utilizada</t>
   </si>
   <si>
-    <t>Indicador: Taxa de mortes violentas Finalidade: Verificar a variação da taxa de mortes violentas Fórmula de cálculo: (Σ de vítimas homicídio doloso + feminicídio + latrocínio + lesão corporal seguida de morte + morte por intervenção policial x 100 mil) /população Periodicidade: Anual Índice Atual de SC 2025: 8,41% (SINESP) Variação (atual/meta): -52,5% Meta 2030 Plano Estadual: 6,0 Fonte: Plano Estadual de Segurança Pública e Defesa Social II de Santa Catarina.</t>
-  </si>
-  <si>
     <t>ESTRATÉGIA DE IMPLEMENTAÇÃO</t>
   </si>
   <si>
@@ -171,9 +165,6 @@
   </si>
   <si>
     <t>A política da Carteira de Políticas do MJSP foi informada? Existe aderência?</t>
-  </si>
-  <si>
-    <t>1 - Reduzir em 20% a taxa de homicídios e feminicídios, latrocínios e lesões corporais seguida de morte nos 60 municípios com população igual ou superior a 26.500 habitantes até 2027</t>
   </si>
   <si>
     <t>SIM</t>
@@ -197,6 +188,75 @@
     </r>
   </si>
   <si>
+    <t>ITENS DE CONTRATAÇÃO</t>
+  </si>
+  <si>
+    <t>Número da Meta Específica</t>
+  </si>
+  <si>
+    <t>Número do Item</t>
+  </si>
+  <si>
+    <t>Ação conforme Art. 7º da portaria nº 685</t>
+  </si>
+  <si>
+    <t>Material/Serviço</t>
+  </si>
+  <si>
+    <t>Instituição</t>
+  </si>
+  <si>
+    <t>Natureza da Despesa</t>
+  </si>
+  <si>
+    <t>Quantidade Planejada</t>
+  </si>
+  <si>
+    <t>Unidade de Medida</t>
+  </si>
+  <si>
+    <t>Valor Planejado Total</t>
+  </si>
+  <si>
+    <t>Status do Item</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">1* </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow (Corpo)"/>
+      </rPr>
+      <t>Redução da taxa estadual de Morte Violenta Intencional para no máximo de 6,41 por 100 mil habitantes até 2027. A taxa atual é de 8,41 mortes por grupo de 100 mil habitantes em 2024, segundo dados do SINESP.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1*</t>
+    </r>
+  </si>
+  <si>
+    <t>0* Indicador: Taxa de mortes violentas Finalidade: Verificar a variação da taxa de mortes violentas Fórmula de cálculo: (Σ de vítimas homicídio doloso + feminicídio + latrocínio + lesão corporal seguida de morte + morte por intervenção policial x 100 mil) /população Periodicidade: Anual Índice Atual de SC 2025: 8,41% (SINESP) Variação (atual/meta): -52,5% Meta 2030 Plano Estadual: 6,0 Fonte: Plano Estadual de Segurança Pública e Defesa Social II de Santa Catarina.0*</t>
+  </si>
+  <si>
+    <t>2*1 - Reduzir em 20% a taxa de homicídios e feminicídios, latrocínios e lesões corporais seguida de morte nos 60 municípios com população igual ou superior a 26.500 habitantes até 2027.2*</t>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">SIM.
 O Indicador e Fórmula de Cálculo informado foi:
@@ -206,12 +266,20 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow (Corpo)"/>
+      </rPr>
+      <t>4*Descrição do Indicador:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
         <rFont val="Aptos Narrow"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">Descrição do Indicador:
-Taxa(%) de ocorrências atendidas
+      <t xml:space="preserve">
+Taxa(%) de ocorrências atendidas.4*
 </t>
     </r>
     <r>
@@ -234,8 +302,8 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">
-Fórmula:
-(Nº de ocorrências atendidas após a aquisição*100 / Nº de ocorrências atendidas realizadasantes da aquisção) - 100.</t>
+5*Fórmula:
+(Nº de ocorrências atendidas após a aquisição*100 / Nº de ocorrências atendidas realizadasantes da aquisção) - 100.5*</t>
     </r>
     <r>
       <rPr>
@@ -263,7 +331,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>1ª Diretriz: Enfrentamento a criminalidade violenta. Ações Estratégicas 1. Redução dos homicídios. Taxa igual ou menor que 6,0/100 mil/hab. até 2030.</t>
+      <t>6*1ª Diretriz: Enfrentamento a criminalidade violenta. Ações Estratégicas 1. Redução dos homicídios. Taxa igual ou menor que 6,0/100 mil/hab. até 2030.6*</t>
     </r>
     <r>
       <rPr>
@@ -291,7 +359,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Meta 1: Reduzir a taxa nacional de homicídios para abaixo de 16 mortes por 100 mil habitantes até 2030</t>
+      <t>7*Meta 1: Reduzir a taxa nacional de homicídios para abaixo de 16 mortes por 100 mil habitantes até 2030.7*</t>
     </r>
     <r>
       <rPr>
@@ -319,7 +387,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Política de Enfrentamento da Criminalidade Violenta</t>
+      <t>8*Política de Enfrentamento da Criminalidade Violenta.8*</t>
     </r>
     <r>
       <rPr>
@@ -333,48 +401,12 @@
 Existe aderência da referida Meta Específica à Política informada.</t>
     </r>
   </si>
-  <si>
-    <t>2 - Reduzir em 20% a taxa de homicídios e feminicídios, latrocínios e lesões corporais seguida de morte nos 60 municípios com população igual ou superior a 26.500 habitantes até 2027</t>
-  </si>
-  <si>
-    <t>ITENS DE CONTRATAÇÃO</t>
-  </si>
-  <si>
-    <t>Número da Meta Específica</t>
-  </si>
-  <si>
-    <t>Número do Item</t>
-  </si>
-  <si>
-    <t>Ação conforme Art. 7º da portaria nº 685</t>
-  </si>
-  <si>
-    <t>Material/Serviço</t>
-  </si>
-  <si>
-    <t>Instituição</t>
-  </si>
-  <si>
-    <t>Natureza da Despesa</t>
-  </si>
-  <si>
-    <t>Quantidade Planejada</t>
-  </si>
-  <si>
-    <t>Unidade de Medida</t>
-  </si>
-  <si>
-    <t>Valor Planejado Total</t>
-  </si>
-  <si>
-    <t>Status do Item</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -408,6 +440,11 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow (Corpo)"/>
     </font>
   </fonts>
   <fills count="6">
@@ -493,7 +530,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -519,22 +556,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -872,8 +912,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J138"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -892,21 +932,21 @@
   <sheetData>
     <row r="1" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
-      <c r="J2" s="11"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="12"/>
     </row>
     <row r="3" spans="1:10" ht="66" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="12" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="6" t="s">
@@ -921,16 +961,16 @@
       <c r="E3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="F3" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11"/>
-      <c r="I3" s="11"/>
-      <c r="J3" s="11"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="12"/>
+      <c r="J3" s="12"/>
     </row>
     <row r="4" spans="1:10" ht="80" x14ac:dyDescent="0.2">
-      <c r="A4" s="11"/>
+      <c r="A4" s="12"/>
       <c r="B4" s="7"/>
       <c r="C4" s="7"/>
       <c r="D4" s="8" t="s">
@@ -939,47 +979,47 @@
       <c r="E4" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="F4" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="9"/>
-      <c r="J4" s="9"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="13"/>
+      <c r="J4" s="13"/>
     </row>
     <row r="5" spans="1:10" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11" t="s">
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="11"/>
-      <c r="I5" s="11"/>
-      <c r="J5" s="11"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="12"/>
     </row>
     <row r="6" spans="1:10" ht="60" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="11"/>
-      <c r="B6" s="9" t="s">
+      <c r="A6" s="12"/>
+      <c r="B6" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9" t="s">
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
-      <c r="I6" s="9"/>
-      <c r="J6" s="9"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="13"/>
     </row>
     <row r="7" spans="1:10" ht="75.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
@@ -997,114 +1037,114 @@
       <c r="E7" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="F7" s="11" t="s">
+      <c r="F7" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="G7" s="11"/>
-      <c r="H7" s="11"/>
-      <c r="I7" s="11"/>
-      <c r="J7" s="11"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="12"/>
+      <c r="J7" s="12"/>
     </row>
     <row r="8" spans="1:10" ht="148.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="B8" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="C8" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="D8" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="D8" s="9" t="s">
+      <c r="E8" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="E8" s="9" t="s">
+      <c r="F8" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="F8" s="9" t="s">
+      <c r="G8" s="13"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="13"/>
+      <c r="J8" s="13"/>
+    </row>
+    <row r="9" spans="1:10" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="13"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="9"/>
-      <c r="J8" s="9"/>
-    </row>
-    <row r="9" spans="1:10" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="9"/>
-      <c r="B9" s="9"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="11" t="s">
+      <c r="G9" s="12"/>
+      <c r="H9" s="12"/>
+      <c r="I9" s="12"/>
+      <c r="J9" s="12"/>
+    </row>
+    <row r="10" spans="1:10" ht="105" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="13"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="G10" s="14"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="14"/>
+      <c r="J10" s="14"/>
+    </row>
+    <row r="11" spans="1:10" ht="114" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="G9" s="11"/>
-      <c r="H9" s="11"/>
-      <c r="I9" s="11"/>
-      <c r="J9" s="11"/>
-    </row>
-    <row r="10" spans="1:10" ht="105" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="9"/>
-      <c r="B10" s="9"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="15" t="s">
+      <c r="B11" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="G10" s="15"/>
-      <c r="H10" s="15"/>
-      <c r="I10" s="15"/>
-      <c r="J10" s="15"/>
-    </row>
-    <row r="11" spans="1:10" ht="114" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="11" t="s">
+      <c r="C11" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="D11" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="E11" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="12"/>
+      <c r="J11" s="12"/>
+    </row>
+    <row r="12" spans="1:10" ht="180.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="12"/>
+      <c r="B12" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="E11" s="11" t="s">
+      <c r="C12" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="F11" s="11"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="11"/>
-      <c r="I11" s="11"/>
-      <c r="J11" s="11"/>
-    </row>
-    <row r="12" spans="1:10" ht="180.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="11"/>
-      <c r="B12" s="8" t="s">
+      <c r="D12" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="E12" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="D12" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="E12" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="9"/>
-      <c r="I12" s="9"/>
-      <c r="J12" s="9"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="13"/>
+      <c r="I12" s="13"/>
+      <c r="J12" s="13"/>
     </row>
     <row r="13" spans="1:10" ht="105.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C13" s="6" t="s">
         <v>17</v>
@@ -1113,368 +1153,350 @@
         <v>18</v>
       </c>
       <c r="E13" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="G13" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="F13" s="6" t="s">
+      <c r="H13" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="G13" s="6" t="s">
+      <c r="I13" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="H13" s="6" t="s">
+      <c r="J13" s="12"/>
+    </row>
+    <row r="14" spans="1:10" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="B14" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="I13" s="11" t="s">
+      <c r="C14" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="E14" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="J13" s="11"/>
-    </row>
-    <row r="14" spans="1:10" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="10" t="s">
+      <c r="F14" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="G14" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="H14" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="I14" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="J14" s="13"/>
+    </row>
+    <row r="15" spans="1:10" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="15"/>
+      <c r="B15" s="13"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
+      <c r="H15" s="13"/>
+      <c r="I15" s="13"/>
+      <c r="J15" s="13"/>
+    </row>
+    <row r="16" spans="1:10" ht="60" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="15"/>
+      <c r="B16" s="13"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="13"/>
+      <c r="H16" s="13"/>
+      <c r="I16" s="13"/>
+      <c r="J16" s="13"/>
+    </row>
+    <row r="17" spans="1:10" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="15"/>
+      <c r="B17" s="13"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
+      <c r="H17" s="13"/>
+      <c r="I17" s="13"/>
+      <c r="J17" s="13"/>
+    </row>
+    <row r="18" spans="1:10" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="15"/>
+      <c r="B18" s="13"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
+      <c r="H18" s="13"/>
+      <c r="I18" s="13"/>
+      <c r="J18" s="13"/>
+    </row>
+    <row r="19" spans="1:10" ht="150" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="15"/>
+      <c r="B19" s="13"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
+      <c r="H19" s="13"/>
+      <c r="I19" s="13"/>
+      <c r="J19" s="13"/>
+    </row>
+    <row r="20" spans="1:10" ht="120" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="15"/>
+      <c r="B20" s="13"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="13"/>
+      <c r="H20" s="13"/>
+      <c r="I20" s="13"/>
+      <c r="J20" s="13"/>
+    </row>
+    <row r="21" spans="1:10" ht="90" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="15"/>
+      <c r="B21" s="13"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="13"/>
+      <c r="H21" s="13"/>
+      <c r="I21" s="13"/>
+      <c r="J21" s="13"/>
+    </row>
+    <row r="22" spans="1:10" ht="60" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="15"/>
+      <c r="B22" s="13"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="13"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="13"/>
+      <c r="G22" s="13"/>
+      <c r="H22" s="13"/>
+      <c r="I22" s="13"/>
+      <c r="J22" s="13"/>
+    </row>
+    <row r="23" spans="1:10" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="15"/>
+      <c r="B23" s="13"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="13"/>
+      <c r="G23" s="13"/>
+      <c r="H23" s="13"/>
+      <c r="I23" s="13"/>
+      <c r="J23" s="13"/>
+    </row>
+    <row r="24" spans="1:10" ht="152" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="15"/>
+      <c r="B24" s="13"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="13"/>
+      <c r="E24" s="13"/>
+      <c r="F24" s="13"/>
+      <c r="G24" s="13"/>
+      <c r="H24" s="13"/>
+      <c r="I24" s="13"/>
+      <c r="J24" s="13"/>
+    </row>
+    <row r="25" spans="1:10" ht="19.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="15"/>
+      <c r="B25" s="13"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="13"/>
+      <c r="F25" s="13"/>
+      <c r="G25" s="13"/>
+      <c r="H25" s="13"/>
+      <c r="I25" s="13"/>
+      <c r="J25" s="13"/>
+    </row>
+    <row r="26" spans="1:10" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="15"/>
+      <c r="B26" s="13"/>
+      <c r="C26" s="13"/>
+      <c r="D26" s="13"/>
+      <c r="E26" s="13"/>
+      <c r="F26" s="13"/>
+      <c r="G26" s="13"/>
+      <c r="H26" s="13"/>
+      <c r="I26" s="13"/>
+      <c r="J26" s="13"/>
+    </row>
+    <row r="27" spans="1:10" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="15"/>
+      <c r="B27" s="13"/>
+      <c r="C27" s="13"/>
+      <c r="D27" s="13"/>
+      <c r="E27" s="13"/>
+      <c r="F27" s="13"/>
+      <c r="G27" s="13"/>
+      <c r="H27" s="13"/>
+      <c r="I27" s="13"/>
+      <c r="J27" s="13"/>
+    </row>
+    <row r="28" spans="1:10" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="15"/>
+      <c r="B28" s="13"/>
+      <c r="C28" s="13"/>
+      <c r="D28" s="13"/>
+      <c r="E28" s="13"/>
+      <c r="F28" s="13"/>
+      <c r="G28" s="13"/>
+      <c r="H28" s="13"/>
+      <c r="I28" s="13"/>
+      <c r="J28" s="13"/>
+    </row>
+    <row r="29" spans="1:10" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="15"/>
+      <c r="B29" s="13"/>
+      <c r="C29" s="13"/>
+      <c r="D29" s="13"/>
+      <c r="E29" s="13"/>
+      <c r="F29" s="13"/>
+      <c r="G29" s="13"/>
+      <c r="H29" s="13"/>
+      <c r="I29" s="13"/>
+      <c r="J29" s="13"/>
+    </row>
+    <row r="30" spans="1:10" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="15"/>
+      <c r="B30" s="13"/>
+      <c r="C30" s="13"/>
+      <c r="D30" s="13"/>
+      <c r="E30" s="13"/>
+      <c r="F30" s="13"/>
+      <c r="G30" s="13"/>
+      <c r="H30" s="13"/>
+      <c r="I30" s="13"/>
+      <c r="J30" s="13"/>
+    </row>
+    <row r="31" spans="1:10" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="15"/>
+      <c r="B31" s="13"/>
+      <c r="C31" s="13"/>
+      <c r="D31" s="13"/>
+      <c r="E31" s="13"/>
+      <c r="F31" s="13"/>
+      <c r="G31" s="13"/>
+      <c r="H31" s="13"/>
+      <c r="I31" s="13"/>
+      <c r="J31" s="13"/>
+    </row>
+    <row r="32" spans="1:10" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="15"/>
+      <c r="B32" s="13"/>
+      <c r="C32" s="13"/>
+      <c r="D32" s="13"/>
+      <c r="E32" s="13"/>
+      <c r="F32" s="13"/>
+      <c r="G32" s="13"/>
+      <c r="H32" s="13"/>
+      <c r="I32" s="13"/>
+      <c r="J32" s="13"/>
+    </row>
+    <row r="33" spans="1:10" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="15"/>
+      <c r="B33" s="13"/>
+      <c r="C33" s="13"/>
+      <c r="D33" s="13"/>
+      <c r="E33" s="13"/>
+      <c r="F33" s="13"/>
+      <c r="G33" s="13"/>
+      <c r="H33" s="13"/>
+      <c r="I33" s="13"/>
+      <c r="J33" s="13"/>
+    </row>
+    <row r="34" spans="1:10" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="15"/>
+      <c r="B34" s="13"/>
+      <c r="C34" s="13"/>
+      <c r="D34" s="13"/>
+      <c r="E34" s="13"/>
+      <c r="F34" s="13"/>
+      <c r="G34" s="13"/>
+      <c r="H34" s="13"/>
+      <c r="I34" s="13"/>
+      <c r="J34" s="13"/>
+    </row>
+    <row r="35" spans="1:10" ht="205" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="15"/>
+      <c r="B35" s="13"/>
+      <c r="C35" s="13"/>
+      <c r="D35" s="13"/>
+      <c r="E35" s="13"/>
+      <c r="F35" s="13"/>
+      <c r="G35" s="13"/>
+      <c r="H35" s="13"/>
+      <c r="I35" s="13"/>
+      <c r="J35" s="13"/>
+    </row>
+    <row r="36" spans="1:10" ht="16" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="37" spans="1:10" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="38" spans="1:10" ht="17" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="B14" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="C14" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="D14" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="E14" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="F14" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="G14" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="H14" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="I14" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="J14" s="9"/>
-    </row>
-    <row r="15" spans="1:10" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="10"/>
-      <c r="B15" s="9"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="9"/>
-      <c r="H15" s="9"/>
-      <c r="I15" s="9"/>
-      <c r="J15" s="9"/>
-    </row>
-    <row r="16" spans="1:10" ht="60" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="10"/>
-      <c r="B16" s="9"/>
-      <c r="C16" s="9"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="9"/>
-      <c r="F16" s="9"/>
-      <c r="G16" s="9"/>
-      <c r="H16" s="9"/>
-      <c r="I16" s="9"/>
-      <c r="J16" s="9"/>
-    </row>
-    <row r="17" spans="1:10" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="10"/>
-      <c r="B17" s="9"/>
-      <c r="C17" s="9"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="9"/>
-      <c r="G17" s="9"/>
-      <c r="H17" s="9"/>
-      <c r="I17" s="9"/>
-      <c r="J17" s="9"/>
-    </row>
-    <row r="18" spans="1:10" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="10"/>
-      <c r="B18" s="9"/>
-      <c r="C18" s="9"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="9"/>
-      <c r="F18" s="9"/>
-      <c r="G18" s="9"/>
-      <c r="H18" s="9"/>
-      <c r="I18" s="9"/>
-      <c r="J18" s="9"/>
-    </row>
-    <row r="19" spans="1:10" ht="150" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="10"/>
-      <c r="B19" s="9"/>
-      <c r="C19" s="9"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
-      <c r="G19" s="9"/>
-      <c r="H19" s="9"/>
-      <c r="I19" s="9"/>
-      <c r="J19" s="9"/>
-    </row>
-    <row r="20" spans="1:10" ht="120" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="10"/>
-      <c r="B20" s="9"/>
-      <c r="C20" s="9"/>
-      <c r="D20" s="9"/>
-      <c r="E20" s="9"/>
-      <c r="F20" s="9"/>
-      <c r="G20" s="9"/>
-      <c r="H20" s="9"/>
-      <c r="I20" s="9"/>
-      <c r="J20" s="9"/>
-    </row>
-    <row r="21" spans="1:10" ht="90" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="10"/>
-      <c r="B21" s="9"/>
-      <c r="C21" s="9"/>
-      <c r="D21" s="9"/>
-      <c r="E21" s="9"/>
-      <c r="F21" s="9"/>
-      <c r="G21" s="9"/>
-      <c r="H21" s="9"/>
-      <c r="I21" s="9"/>
-      <c r="J21" s="9"/>
-    </row>
-    <row r="22" spans="1:10" ht="60" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="10"/>
-      <c r="B22" s="9"/>
-      <c r="C22" s="9"/>
-      <c r="D22" s="9"/>
-      <c r="E22" s="9"/>
-      <c r="F22" s="9"/>
-      <c r="G22" s="9"/>
-      <c r="H22" s="9"/>
-      <c r="I22" s="9"/>
-      <c r="J22" s="9"/>
-    </row>
-    <row r="23" spans="1:10" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="10"/>
-      <c r="B23" s="9"/>
-      <c r="C23" s="9"/>
-      <c r="D23" s="9"/>
-      <c r="E23" s="9"/>
-      <c r="F23" s="9"/>
-      <c r="G23" s="9"/>
-      <c r="H23" s="9"/>
-      <c r="I23" s="9"/>
-      <c r="J23" s="9"/>
-    </row>
-    <row r="24" spans="1:10" ht="120" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="10"/>
-      <c r="B24" s="9"/>
-      <c r="C24" s="9"/>
-      <c r="D24" s="9"/>
-      <c r="E24" s="9"/>
-      <c r="F24" s="9"/>
-      <c r="G24" s="9"/>
-      <c r="H24" s="9"/>
-      <c r="I24" s="9"/>
-      <c r="J24" s="9"/>
-    </row>
-    <row r="25" spans="1:10" ht="19.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="B25" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="C25" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="D25" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="E25" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="F25" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="G25" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="H25" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="I25" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="J25" s="9"/>
-    </row>
-    <row r="26" spans="1:10" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="10"/>
-      <c r="B26" s="9"/>
-      <c r="C26" s="9"/>
-      <c r="D26" s="9"/>
-      <c r="E26" s="9"/>
-      <c r="F26" s="9"/>
-      <c r="G26" s="9"/>
-      <c r="H26" s="9"/>
-      <c r="I26" s="9"/>
-      <c r="J26" s="9"/>
-    </row>
-    <row r="27" spans="1:10" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="10"/>
-      <c r="B27" s="9"/>
-      <c r="C27" s="9"/>
-      <c r="D27" s="9"/>
-      <c r="E27" s="9"/>
-      <c r="F27" s="9"/>
-      <c r="G27" s="9"/>
-      <c r="H27" s="9"/>
-      <c r="I27" s="9"/>
-      <c r="J27" s="9"/>
-    </row>
-    <row r="28" spans="1:10" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="10"/>
-      <c r="B28" s="9"/>
-      <c r="C28" s="9"/>
-      <c r="D28" s="9"/>
-      <c r="E28" s="9"/>
-      <c r="F28" s="9"/>
-      <c r="G28" s="9"/>
-      <c r="H28" s="9"/>
-      <c r="I28" s="9"/>
-      <c r="J28" s="9"/>
-    </row>
-    <row r="29" spans="1:10" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="10"/>
-      <c r="B29" s="9"/>
-      <c r="C29" s="9"/>
-      <c r="D29" s="9"/>
-      <c r="E29" s="9"/>
-      <c r="F29" s="9"/>
-      <c r="G29" s="9"/>
-      <c r="H29" s="9"/>
-      <c r="I29" s="9"/>
-      <c r="J29" s="9"/>
-    </row>
-    <row r="30" spans="1:10" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="10"/>
-      <c r="B30" s="9"/>
-      <c r="C30" s="9"/>
-      <c r="D30" s="9"/>
-      <c r="E30" s="9"/>
-      <c r="F30" s="9"/>
-      <c r="G30" s="9"/>
-      <c r="H30" s="9"/>
-      <c r="I30" s="9"/>
-      <c r="J30" s="9"/>
-    </row>
-    <row r="31" spans="1:10" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="10"/>
-      <c r="B31" s="9"/>
-      <c r="C31" s="9"/>
-      <c r="D31" s="9"/>
-      <c r="E31" s="9"/>
-      <c r="F31" s="9"/>
-      <c r="G31" s="9"/>
-      <c r="H31" s="9"/>
-      <c r="I31" s="9"/>
-      <c r="J31" s="9"/>
-    </row>
-    <row r="32" spans="1:10" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="10"/>
-      <c r="B32" s="9"/>
-      <c r="C32" s="9"/>
-      <c r="D32" s="9"/>
-      <c r="E32" s="9"/>
-      <c r="F32" s="9"/>
-      <c r="G32" s="9"/>
-      <c r="H32" s="9"/>
-      <c r="I32" s="9"/>
-      <c r="J32" s="9"/>
-    </row>
-    <row r="33" spans="1:10" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="10"/>
-      <c r="B33" s="9"/>
-      <c r="C33" s="9"/>
-      <c r="D33" s="9"/>
-      <c r="E33" s="9"/>
-      <c r="F33" s="9"/>
-      <c r="G33" s="9"/>
-      <c r="H33" s="9"/>
-      <c r="I33" s="9"/>
-      <c r="J33" s="9"/>
-    </row>
-    <row r="34" spans="1:10" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="10"/>
-      <c r="B34" s="9"/>
-      <c r="C34" s="9"/>
-      <c r="D34" s="9"/>
-      <c r="E34" s="9"/>
-      <c r="F34" s="9"/>
-      <c r="G34" s="9"/>
-      <c r="H34" s="9"/>
-      <c r="I34" s="9"/>
-      <c r="J34" s="9"/>
-    </row>
-    <row r="35" spans="1:10" ht="192" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="10"/>
-      <c r="B35" s="9"/>
-      <c r="C35" s="9"/>
-      <c r="D35" s="9"/>
-      <c r="E35" s="9"/>
-      <c r="F35" s="9"/>
-      <c r="G35" s="9"/>
-      <c r="H35" s="9"/>
-      <c r="I35" s="9"/>
-      <c r="J35" s="9"/>
-    </row>
-    <row r="36" spans="1:10" ht="16" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="37" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="38" spans="1:10" ht="17" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="B38" s="13"/>
-      <c r="C38" s="13"/>
-      <c r="D38" s="13"/>
-      <c r="E38" s="13"/>
-      <c r="F38" s="13"/>
-      <c r="G38" s="13"/>
-      <c r="H38" s="13"/>
-      <c r="I38" s="13"/>
-      <c r="J38" s="14"/>
+      <c r="B38" s="10"/>
+      <c r="C38" s="10"/>
+      <c r="D38" s="10"/>
+      <c r="E38" s="10"/>
+      <c r="F38" s="10"/>
+      <c r="G38" s="10"/>
+      <c r="H38" s="10"/>
+      <c r="I38" s="10"/>
+      <c r="J38" s="11"/>
     </row>
     <row r="39" spans="1:10" ht="50" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="I39" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="J39" s="1" t="s">
         <v>55</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="E39" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="F39" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="G39" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="H39" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="I39" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="J39" s="1" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="40" spans="1:10" ht="222" customHeight="1" x14ac:dyDescent="0.2">
@@ -2656,6 +2678,31 @@
     <row r="138" spans="1:10" ht="16" customHeight="1" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="41">
+    <mergeCell ref="F25:F35"/>
+    <mergeCell ref="G25:G35"/>
+    <mergeCell ref="H25:H35"/>
+    <mergeCell ref="I25:J35"/>
+    <mergeCell ref="A25:A35"/>
+    <mergeCell ref="B25:B35"/>
+    <mergeCell ref="C25:C35"/>
+    <mergeCell ref="D25:D35"/>
+    <mergeCell ref="E25:E35"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="A14:A24"/>
+    <mergeCell ref="B14:B24"/>
+    <mergeCell ref="C14:C24"/>
+    <mergeCell ref="D14:D24"/>
+    <mergeCell ref="I13:J13"/>
+    <mergeCell ref="E14:E24"/>
+    <mergeCell ref="F14:F24"/>
+    <mergeCell ref="G14:G24"/>
+    <mergeCell ref="H14:H24"/>
+    <mergeCell ref="I14:J24"/>
+    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="D8:D10"/>
+    <mergeCell ref="E8:E10"/>
+    <mergeCell ref="E11:J11"/>
+    <mergeCell ref="E12:J12"/>
     <mergeCell ref="A38:J38"/>
     <mergeCell ref="A2:J2"/>
     <mergeCell ref="F3:J3"/>
@@ -2672,31 +2719,6 @@
     <mergeCell ref="B6:D6"/>
     <mergeCell ref="A8:A10"/>
     <mergeCell ref="B8:B10"/>
-    <mergeCell ref="C8:C10"/>
-    <mergeCell ref="D8:D10"/>
-    <mergeCell ref="E8:E10"/>
-    <mergeCell ref="E11:J11"/>
-    <mergeCell ref="E12:J12"/>
-    <mergeCell ref="I13:J13"/>
-    <mergeCell ref="E14:E24"/>
-    <mergeCell ref="F14:F24"/>
-    <mergeCell ref="G14:G24"/>
-    <mergeCell ref="H14:H24"/>
-    <mergeCell ref="I14:J24"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="A14:A24"/>
-    <mergeCell ref="B14:B24"/>
-    <mergeCell ref="C14:C24"/>
-    <mergeCell ref="D14:D24"/>
-    <mergeCell ref="F25:F35"/>
-    <mergeCell ref="G25:G35"/>
-    <mergeCell ref="H25:H35"/>
-    <mergeCell ref="I25:J35"/>
-    <mergeCell ref="A25:A35"/>
-    <mergeCell ref="B25:B35"/>
-    <mergeCell ref="C25:C35"/>
-    <mergeCell ref="D25:D35"/>
-    <mergeCell ref="E25:E35"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>